<commit_message>
Repaired 3c; the flip-flop now correctly switches on low clock signal
</commit_message>
<xml_diff>
--- a/Lab3/3c_syncJK_tabela.xlsx
+++ b/Lab3/3c_syncJK_tabela.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Dropbox\Studia\Technika Cyfrowa\cyfrowa\Lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\luknw\studia\03_semestr\TC\cyfrowa\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>J</t>
   </si>
@@ -41,28 +41,7 @@
     <t>~Q(n-1)</t>
   </si>
   <si>
-    <t>Q(n-1)\JK</t>
-  </si>
-  <si>
-    <t>00</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>JQ(n-1)' + K'Q(n-1)</t>
+    <t>Zmiany stanu następują, gdy na wejściu zegarowym jest stan niski.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +131,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -168,9 +147,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +187,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -280,7 +259,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -430,200 +409,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A3:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E9" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -632,8 +547,10 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -642,8 +559,10 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -653,7 +572,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -663,7 +582,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -673,7 +592,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>

</xml_diff>